<commit_message>
Student Added the Abc
</commit_message>
<xml_diff>
--- a/backend/excel/students.xlsx
+++ b/backend/excel/students.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo Tiny PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dir\jssp\backend\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Student Name</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t xml:space="preserve">Division </t>
+  </si>
+  <si>
+    <t>ABC</t>
   </si>
 </sst>
 </file>
@@ -363,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +457,7 @@
     <col min="100" max="100" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,6 +466,9 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>